<commit_message>
added some warband info for kais orks
</commit_message>
<xml_diff>
--- a/mordheim_kai.xlsx
+++ b/mordheim_kai.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\klaute\dev\Mordheim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3800E3F2-7BCD-40F2-A202-348972413A4C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3A5916CF-35A0-4786-972F-850640AD5B22}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>gold</t>
   </si>
@@ -147,21 +147,12 @@
     <t>(alle tragen einen dolch)</t>
   </si>
   <si>
-    <t>armbrust, leichte rüstung</t>
-  </si>
-  <si>
     <t>2 dolche/schwerter</t>
   </si>
   <si>
     <t>2 dolche/äxte/schwerter</t>
   </si>
   <si>
-    <t>3 speere</t>
-  </si>
-  <si>
-    <t>3 dolche/schwerter</t>
-  </si>
-  <si>
     <t>3x Speerträger, 1x 2 Schwert/Axt, 3x 1 Schwert</t>
   </si>
   <si>
@@ -171,28 +162,49 @@
     <t>Ausrüstung</t>
   </si>
   <si>
-    <t>custom boss</t>
-  </si>
-  <si>
-    <t>shaman</t>
-  </si>
-  <si>
-    <t>3 goblin speerträger</t>
-  </si>
-  <si>
-    <t>3 schlitzer goblins</t>
-  </si>
-  <si>
-    <t>1 goblin hero</t>
-  </si>
-  <si>
-    <t>1 narts goblin</t>
+    <t>ork savage boyz</t>
+  </si>
+  <si>
+    <t>1x Goblin Hero (Gamezone)</t>
+  </si>
+  <si>
+    <t>Kosten/Stück</t>
+  </si>
+  <si>
+    <t>1x Nartz (Freebooters Fate)</t>
+  </si>
+  <si>
+    <t>1x 3 Goblin Speerträger (Gamezone)</t>
+  </si>
+  <si>
+    <t>1x Orc Shaman (Avatars of War)</t>
+  </si>
+  <si>
+    <t>3  Fiese Schlitzer (GW)</t>
+  </si>
+  <si>
+    <t>1x custom boss</t>
+  </si>
+  <si>
+    <t>je 1 dolch/schwert</t>
+  </si>
+  <si>
+    <t>je 1 speer 3 schild</t>
+  </si>
+  <si>
+    <t>1x Dämonische Jägerin Banner (Gamezone)</t>
+  </si>
+  <si>
+    <t>für Schamane</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -271,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -279,9 +291,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -583,19 +602,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:O25"/>
+  <dimension ref="A2:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3" bestFit="1" customWidth="1"/>
@@ -606,20 +625,21 @@
     <col min="13" max="13" width="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>43332</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -644,14 +664,23 @@
       <c r="O4" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="4">
         <f>D16+J17+O16</f>
-        <v>290</v>
+        <v>335</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -679,14 +708,24 @@
         <f>N5*M5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="R5" s="11">
+        <v>6.3</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="T5" s="7"/>
+    </row>
+    <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>31</v>
       </c>
       <c r="B6">
         <f>B4-B5</f>
-        <v>210</v>
+        <v>165</v>
       </c>
       <c r="G6" t="s">
         <v>1</v>
@@ -714,8 +753,18 @@
         <f t="shared" ref="O6:O15" si="1">N6*M6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="R6" s="11">
+        <v>10.71</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="T6" s="7"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
         <v>39</v>
       </c>
@@ -745,8 +794,18 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="R7" s="11">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T7" s="7"/>
+    </row>
+    <row r="8" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -785,8 +844,18 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q8" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="R8" s="11">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="T8" s="7"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -810,11 +879,11 @@
         <v>10</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L9" t="s">
         <v>17</v>
@@ -829,8 +898,18 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="R9" s="11">
+        <v>0</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="T9" s="7"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -870,8 +949,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R10" s="11">
+        <v>10.36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -885,9 +970,6 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
       <c r="G11" t="s">
         <v>6</v>
       </c>
@@ -908,14 +990,20 @@
         <v>5</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O11">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="Q11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="R11" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -930,7 +1018,7 @@
         <v>105</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
         <v>7</v>
@@ -958,8 +1046,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="R12" s="11">
+        <v>6.3</v>
+      </c>
+      <c r="S12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1000,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1021,11 +1118,11 @@
         <v>20</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L14" t="s">
         <v>20</v>
@@ -1040,8 +1137,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R14" s="12">
+        <f>SUM(R5:R13)</f>
+        <v>52.069999999999993</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>27</v>
       </c>
@@ -1082,7 +1183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D16" s="1">
         <f>SUM(D9:D15)</f>
         <v>225</v>
@@ -1102,7 +1203,7 @@
       </c>
       <c r="O16" s="1">
         <f>SUM(O5:O15)</f>
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1110,77 +1211,10 @@
       <c r="B17" s="2"/>
       <c r="J17" s="1">
         <f>SUM(J5:J16)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-  </mergeCells>
   <conditionalFormatting sqref="B5">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
       <formula>$B$4</formula>

</xml_diff>